<commit_message>
change StockTable to StockHistory
</commit_message>
<xml_diff>
--- a/docs/table.xlsx
+++ b/docs/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin\home\hishidama\git\tsurugi\cost-accounting-benchmark\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12C3E24-FC01-4DAB-9675-E47CFE3B443D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E072ED3-275D-42D3-9E85-D38698C49ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="2940" windowWidth="27075" windowHeight="18705" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12435" yWindow="3045" windowWidth="27090" windowHeight="18705" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工場" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="品目構成" sheetId="3" r:id="rId3"/>
     <sheet name="製造品目" sheetId="4" r:id="rId4"/>
     <sheet name="原価" sheetId="5" r:id="rId5"/>
-    <sheet name="在庫" sheetId="8" r:id="rId6"/>
+    <sheet name="在庫履歴" sheetId="8" r:id="rId6"/>
     <sheet name="度量衡" sheetId="6" r:id="rId7"/>
     <sheet name="結果" sheetId="7" r:id="rId8"/>
   </sheets>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="165">
   <si>
     <t>工場マスター</t>
   </si>
@@ -479,17 +479,6 @@
   </si>
   <si>
     <t>製造原価×生産数</t>
-  </si>
-  <si>
-    <t>在庫テーブル</t>
-    <rPh sb="0" eb="2">
-      <t>ザイコ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>stock_table</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>s_stock_amount</t>
@@ -521,6 +510,95 @@
   </si>
   <si>
     <t>s_f_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>在庫金額</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>品目ID</t>
+    <rPh sb="0" eb="2">
+      <t>ヒンモク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>stock_history</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>在庫履歴</t>
+    <rPh sb="0" eb="2">
+      <t>ザイコ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>リレキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_i_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時刻</t>
+    <rPh sb="0" eb="2">
+      <t>ジコク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>時分秒</t>
+    <rPh sb="0" eb="3">
+      <t>ジフンビョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>在庫数量</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_stock_unit</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>s_stock_quantity</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>原価マスター．在庫単位</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンカ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ザイコ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>タンイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>原価マスター．在庫数量</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンカ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ザイコ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>スウリョウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1710,7 +1788,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1912,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C235D5-E401-491B-A45B-BE54012A0C8E}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1929,10 +2007,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -1960,7 +2038,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -1974,17 +2052,17 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C4" t="str">
-        <f>工場!C3</f>
+        <f>原価!C3</f>
         <v>unique ID</v>
       </c>
       <c r="D4">
-        <f>工場!D3</f>
+        <f>原価!D3</f>
         <v>4</v>
       </c>
       <c r="F4" t="s">
@@ -1993,78 +2071,159 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="C5" t="str">
+        <f>原価!C4</f>
+        <v>unique ID</v>
+      </c>
+      <c r="D5">
+        <f>原価!D4</f>
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" t="str">
+        <f>原価!C5</f>
+        <v>variable text</v>
+      </c>
+      <c r="D7">
+        <f>原価!D5</f>
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="str">
+        <f>原価!C6</f>
+        <v>unsigned numeric</v>
+      </c>
+      <c r="D8">
+        <f>原価!D6</f>
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <f>原価!E6</f>
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" t="str">
         <f>原価!C7</f>
         <v>unsigned numeric</v>
       </c>
-      <c r="D5">
+      <c r="D9">
         <f>原価!D7</f>
         <v>13</v>
       </c>
-      <c r="E5">
+      <c r="E9">
         <f>原価!E7</f>
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C10" s="1"/>
+      <c r="G9" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="C11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.15">
       <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="C26" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>